<commit_message>
Fixed column headers in spreadsheet and RCode
Now fixed and run!
</commit_message>
<xml_diff>
--- a/GC/cosall.xlsx
+++ b/GC/cosall.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mail\2025\0621\0624New\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgenbauer/Desktop/HCC 25/_GitArchive/MBauer-HCC25/GC/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC436B35-787A-0847-A04F-0CE652F910BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5484"/>
+    <workbookView xWindow="9960" yWindow="1100" windowWidth="20640" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cosall" sheetId="1" r:id="rId1"/>
@@ -47,36 +48,15 @@
     <t>Pvalue</t>
   </si>
   <si>
-    <t>A(overall)</t>
-  </si>
-  <si>
-    <t>ϕ[Orthophase]</t>
-  </si>
-  <si>
-    <t>ϕ[Bathyphase]</t>
-  </si>
-  <si>
     <t>Tau1</t>
   </si>
   <si>
-    <t>PR(Tau1)</t>
-  </si>
-  <si>
-    <t>P(Tau1)</t>
-  </si>
-  <si>
-    <t>A[1]</t>
-  </si>
-  <si>
     <t>SE(A1)</t>
   </si>
   <si>
     <t>A[1,CI95]</t>
   </si>
   <si>
-    <t>Phi(1)</t>
-  </si>
-  <si>
     <t>ϕ[1,SE]</t>
   </si>
   <si>
@@ -86,24 +66,12 @@
     <t>Tau2</t>
   </si>
   <si>
-    <t>PR(Tau2)</t>
-  </si>
-  <si>
-    <t>P(Tau2)</t>
-  </si>
-  <si>
-    <t>A[2]</t>
-  </si>
-  <si>
     <t>A[2,SE]</t>
   </si>
   <si>
     <t>A[2,CI95]</t>
   </si>
   <si>
-    <t>Phi(2)</t>
-  </si>
-  <si>
     <t>ϕ[2,SE]</t>
   </si>
   <si>
@@ -672,12 +640,45 @@
   </si>
   <si>
     <t>HR056b2D</t>
+  </si>
+  <si>
+    <t>PRTau1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>PRTau2</t>
+  </si>
+  <si>
+    <t>Phi1</t>
+  </si>
+  <si>
+    <t>PTau1</t>
+  </si>
+  <si>
+    <t>PTau2</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Phi2</t>
+  </si>
+  <si>
+    <t>ϕOrthophase</t>
+  </si>
+  <si>
+    <t>ϕBathyphase</t>
+  </si>
+  <si>
+    <t>Aoverall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1001,33 +1002,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="8.88671875" style="3"/>
-    <col min="7" max="8" width="8.88671875" style="2"/>
-    <col min="9" max="13" width="8.88671875" style="3"/>
-    <col min="14" max="16" width="8.88671875" style="2"/>
-    <col min="17" max="22" width="8.88671875" style="3"/>
-    <col min="23" max="25" width="8.88671875" style="2"/>
-    <col min="26" max="28" width="8.88671875" style="3"/>
-    <col min="30" max="30" width="8.88671875" style="1"/>
-    <col min="31" max="31" width="5.5546875" style="1" customWidth="1"/>
-    <col min="32" max="34" width="8.88671875" style="1"/>
+    <col min="4" max="5" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="8.83203125" style="3"/>
+    <col min="7" max="8" width="8.83203125" style="2"/>
+    <col min="9" max="13" width="8.83203125" style="3"/>
+    <col min="14" max="16" width="8.83203125" style="2"/>
+    <col min="17" max="22" width="8.83203125" style="3"/>
+    <col min="23" max="25" width="8.83203125" style="2"/>
+    <col min="26" max="28" width="8.83203125" style="3"/>
+    <col min="30" max="30" width="8.83203125" style="1"/>
+    <col min="31" max="31" width="5.5" style="1" customWidth="1"/>
+    <col min="32" max="34" width="8.83203125" style="1"/>
     <col min="35" max="35" width="7.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1050,99 +1051,99 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J1" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="AB1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>137.47479798519399</v>
@@ -1208,7 +1209,7 @@
         <v>34</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD2" s="1">
         <v>2</v>
@@ -1220,18 +1221,18 @@
         <v>0.05</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2">
         <v>138.852427705358</v>
@@ -1297,7 +1298,7 @@
         <v>56</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD3" s="1">
         <v>2</v>
@@ -1309,18 +1310,18 @@
         <v>0.05</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2">
         <v>138.083885250609</v>
@@ -1386,7 +1387,7 @@
         <v>59</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD4" s="1">
         <v>2</v>
@@ -1398,18 +1399,18 @@
         <v>0.05</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2">
         <v>148.63136813570301</v>
@@ -1475,7 +1476,7 @@
         <v>45</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD5" s="1">
         <v>2</v>
@@ -1487,18 +1488,18 @@
         <v>0.05</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>128.45522197669899</v>
@@ -1564,7 +1565,7 @@
         <v>51</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD6" s="1">
         <v>2</v>
@@ -1576,18 +1577,18 @@
         <v>0.05</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2">
         <v>123.651697164013</v>
@@ -1653,7 +1654,7 @@
         <v>29</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD7" s="1">
         <v>2</v>
@@ -1665,18 +1666,18 @@
         <v>0.05</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2">
         <v>135.29489480117201</v>
@@ -1742,7 +1743,7 @@
         <v>63</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD8" s="1">
         <v>2</v>
@@ -1754,18 +1755,18 @@
         <v>0.05</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2">
         <v>131.66132884254901</v>
@@ -1831,7 +1832,7 @@
         <v>124</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD9" s="1">
         <v>2</v>
@@ -1843,18 +1844,18 @@
         <v>0.05</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2">
         <v>130.49263291798599</v>
@@ -1920,7 +1921,7 @@
         <v>46</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD10" s="1">
         <v>2</v>
@@ -1932,18 +1933,18 @@
         <v>0.05</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2">
         <v>128.936055238119</v>
@@ -2009,7 +2010,7 @@
         <v>136</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD11" s="1">
         <v>2</v>
@@ -2021,18 +2022,18 @@
         <v>0.05</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2">
         <v>127.636575859297</v>
@@ -2098,7 +2099,7 @@
         <v>25</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD12" s="1">
         <v>2</v>
@@ -2110,18 +2111,18 @@
         <v>0.05</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2">
         <v>136.922342948042</v>
@@ -2187,7 +2188,7 @@
         <v>32</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD13" s="1">
         <v>2</v>
@@ -2199,18 +2200,18 @@
         <v>0.05</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2">
         <v>129.53429546897499</v>
@@ -2276,7 +2277,7 @@
         <v>40</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD14" s="1">
         <v>2</v>
@@ -2288,18 +2289,18 @@
         <v>0.05</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2">
         <v>130.11575391202601</v>
@@ -2365,7 +2366,7 @@
         <v>79</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD15" s="1">
         <v>2</v>
@@ -2377,18 +2378,18 @@
         <v>0.05</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D16" s="2">
         <v>154.72335589818701</v>
@@ -2454,7 +2455,7 @@
         <v>24</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD16" s="1">
         <v>2</v>
@@ -2466,18 +2467,18 @@
         <v>0.05</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2">
         <v>150.00460678649199</v>
@@ -2543,7 +2544,7 @@
         <v>99</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD17" s="1">
         <v>2</v>
@@ -2555,18 +2556,18 @@
         <v>0.05</v>
       </c>
       <c r="AI17" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2">
         <v>142.471713427791</v>
@@ -2632,7 +2633,7 @@
         <v>33</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD18" s="1">
         <v>2</v>
@@ -2644,18 +2645,18 @@
         <v>0.05</v>
       </c>
       <c r="AI18" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D19" s="2">
         <v>136.80820527120599</v>
@@ -2721,7 +2722,7 @@
         <v>58</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD19" s="1">
         <v>2</v>
@@ -2733,18 +2734,18 @@
         <v>0.05</v>
       </c>
       <c r="AI19" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2">
         <v>137.56517661509099</v>
@@ -2810,7 +2811,7 @@
         <v>41</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD20" s="1">
         <v>2</v>
@@ -2822,18 +2823,18 @@
         <v>0.05</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D21" s="2">
         <v>128.98439899001701</v>
@@ -2899,7 +2900,7 @@
         <v>36</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD21" s="1">
         <v>2</v>
@@ -2911,18 +2912,18 @@
         <v>0.05</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2">
         <v>148.363964592683</v>
@@ -2988,7 +2989,7 @@
         <v>21</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD22" s="1">
         <v>2</v>
@@ -3000,18 +3001,18 @@
         <v>0.05</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2">
         <v>142.843578554869</v>
@@ -3077,7 +3078,7 @@
         <v>19</v>
       </c>
       <c r="AC23" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD23" s="1">
         <v>2</v>
@@ -3089,18 +3090,18 @@
         <v>0.05</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D24" s="2">
         <v>145.766519068126</v>
@@ -3166,7 +3167,7 @@
         <v>66</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD24" s="1">
         <v>2</v>
@@ -3178,18 +3179,18 @@
         <v>0.05</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D25" s="2">
         <v>138.12321595213899</v>
@@ -3255,7 +3256,7 @@
         <v>30</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD25" s="1">
         <v>2</v>
@@ -3267,18 +3268,18 @@
         <v>0.05</v>
       </c>
       <c r="AI25" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D26" s="2">
         <v>159.93496089812299</v>
@@ -3344,7 +3345,7 @@
         <v>52</v>
       </c>
       <c r="AC26" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD26" s="1">
         <v>2</v>
@@ -3356,18 +3357,18 @@
         <v>0.05</v>
       </c>
       <c r="AI26" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D27" s="2">
         <v>161.33147716551801</v>
@@ -3433,7 +3434,7 @@
         <v>219</v>
       </c>
       <c r="AC27" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD27" s="1">
         <v>2</v>
@@ -3445,18 +3446,18 @@
         <v>0.05</v>
       </c>
       <c r="AI27" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D28" s="2">
         <v>130.67618815128299</v>
@@ -3522,7 +3523,7 @@
         <v>191</v>
       </c>
       <c r="AC28" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD28" s="1">
         <v>2</v>
@@ -3534,18 +3535,18 @@
         <v>0.05</v>
       </c>
       <c r="AI28" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2">
         <v>137.60268991637</v>
@@ -3611,7 +3612,7 @@
         <v>86</v>
       </c>
       <c r="AC29" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD29" s="1">
         <v>2</v>
@@ -3623,18 +3624,18 @@
         <v>0.05</v>
       </c>
       <c r="AI29" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D30" s="2">
         <v>136.37682136193499</v>
@@ -3700,7 +3701,7 @@
         <v>19</v>
       </c>
       <c r="AC30" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD30" s="1">
         <v>2</v>
@@ -3712,18 +3713,18 @@
         <v>0.05</v>
       </c>
       <c r="AI30" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D31" s="2">
         <v>139.91256073403301</v>
@@ -3789,7 +3790,7 @@
         <v>41</v>
       </c>
       <c r="AC31" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD31" s="1">
         <v>2</v>
@@ -3801,18 +3802,18 @@
         <v>0.05</v>
       </c>
       <c r="AI31" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D32" s="2">
         <v>132.39408308550099</v>
@@ -3878,7 +3879,7 @@
         <v>32</v>
       </c>
       <c r="AC32" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD32" s="1">
         <v>2</v>
@@ -3890,18 +3891,18 @@
         <v>0.05</v>
       </c>
       <c r="AI32" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2">
         <v>125.48622077479401</v>
@@ -3967,7 +3968,7 @@
         <v>33</v>
       </c>
       <c r="AC33" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD33" s="1">
         <v>2</v>
@@ -3979,18 +3980,18 @@
         <v>0.05</v>
       </c>
       <c r="AI33" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D34" s="2">
         <v>150.86948567927999</v>
@@ -4056,7 +4057,7 @@
         <v>27</v>
       </c>
       <c r="AC34" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD34" s="1">
         <v>2</v>
@@ -4068,18 +4069,18 @@
         <v>0.05</v>
       </c>
       <c r="AI34" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D35" s="2">
         <v>125.23096641684</v>
@@ -4145,7 +4146,7 @@
         <v>46</v>
       </c>
       <c r="AC35" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD35" s="1">
         <v>2</v>
@@ -4157,18 +4158,18 @@
         <v>0.05</v>
       </c>
       <c r="AI35" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D36" s="2">
         <v>131.931707228791</v>
@@ -4234,7 +4235,7 @@
         <v>58</v>
       </c>
       <c r="AC36" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD36" s="1">
         <v>2</v>
@@ -4246,18 +4247,18 @@
         <v>0.05</v>
       </c>
       <c r="AI36" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D37" s="2">
         <v>135.96327218762801</v>
@@ -4323,7 +4324,7 @@
         <v>56</v>
       </c>
       <c r="AC37" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD37" s="1">
         <v>2</v>
@@ -4335,18 +4336,18 @@
         <v>0.05</v>
       </c>
       <c r="AI37" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D38" s="2">
         <v>140.083245332827</v>
@@ -4412,7 +4413,7 @@
         <v>48</v>
       </c>
       <c r="AC38" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD38" s="1">
         <v>2</v>
@@ -4424,18 +4425,18 @@
         <v>0.05</v>
       </c>
       <c r="AI38" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D39" s="2">
         <v>129.25509708176</v>
@@ -4501,7 +4502,7 @@
         <v>106</v>
       </c>
       <c r="AC39" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD39" s="1">
         <v>2</v>
@@ -4513,18 +4514,18 @@
         <v>0.05</v>
       </c>
       <c r="AI39" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D40" s="2">
         <v>134.93995114092101</v>
@@ -4590,7 +4591,7 @@
         <v>38</v>
       </c>
       <c r="AC40" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD40" s="1">
         <v>2</v>
@@ -4602,18 +4603,18 @@
         <v>0.05</v>
       </c>
       <c r="AI40" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D41" s="2">
         <v>125.642656905507</v>
@@ -4679,7 +4680,7 @@
         <v>33</v>
       </c>
       <c r="AC41" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD41" s="1">
         <v>2</v>
@@ -4691,18 +4692,18 @@
         <v>0.05</v>
       </c>
       <c r="AI41" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D42" s="2">
         <v>141.779952291949</v>
@@ -4768,7 +4769,7 @@
         <v>37</v>
       </c>
       <c r="AC42" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD42" s="1">
         <v>2</v>
@@ -4780,18 +4781,18 @@
         <v>0.05</v>
       </c>
       <c r="AI42" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D43" s="2">
         <v>144.019979395219</v>
@@ -4857,7 +4858,7 @@
         <v>38</v>
       </c>
       <c r="AC43" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD43" s="1">
         <v>2</v>
@@ -4869,18 +4870,18 @@
         <v>0.05</v>
       </c>
       <c r="AI43" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D44" s="2">
         <v>116.924815652889</v>
@@ -4946,7 +4947,7 @@
         <v>79</v>
       </c>
       <c r="AC44" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD44" s="1">
         <v>2</v>
@@ -4958,18 +4959,18 @@
         <v>0.05</v>
       </c>
       <c r="AI44" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D45" s="2">
         <v>112.975751315707</v>
@@ -5035,7 +5036,7 @@
         <v>116</v>
       </c>
       <c r="AC45" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD45" s="1">
         <v>2</v>
@@ -5047,18 +5048,18 @@
         <v>0.05</v>
       </c>
       <c r="AI45" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D46" s="2">
         <v>135.48687184919399</v>
@@ -5124,7 +5125,7 @@
         <v>26</v>
       </c>
       <c r="AC46" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD46" s="1">
         <v>2</v>
@@ -5136,18 +5137,18 @@
         <v>0.05</v>
       </c>
       <c r="AI46" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D47" s="2">
         <v>148.71013223653</v>
@@ -5213,7 +5214,7 @@
         <v>38</v>
       </c>
       <c r="AC47" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD47" s="1">
         <v>2</v>
@@ -5225,18 +5226,18 @@
         <v>0.05</v>
       </c>
       <c r="AI47" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D48" s="2">
         <v>130.53986331976299</v>
@@ -5302,7 +5303,7 @@
         <v>140</v>
       </c>
       <c r="AC48" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD48" s="1">
         <v>2</v>
@@ -5314,18 +5315,18 @@
         <v>0.05</v>
       </c>
       <c r="AI48" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D49" s="2">
         <v>129.01730089028101</v>
@@ -5391,7 +5392,7 @@
         <v>18</v>
       </c>
       <c r="AC49" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD49" s="1">
         <v>2</v>
@@ -5403,18 +5404,18 @@
         <v>0.05</v>
       </c>
       <c r="AI49" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D50" s="2">
         <v>144.50103417819599</v>
@@ -5480,7 +5481,7 @@
         <v>51</v>
       </c>
       <c r="AC50" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD50" s="1">
         <v>2</v>
@@ -5492,18 +5493,18 @@
         <v>0.05</v>
       </c>
       <c r="AI50" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D51" s="2">
         <v>141.53894696972</v>
@@ -5569,7 +5570,7 @@
         <v>18</v>
       </c>
       <c r="AC51" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD51" s="1">
         <v>2</v>
@@ -5581,18 +5582,18 @@
         <v>0.05</v>
       </c>
       <c r="AI51" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D52" s="2">
         <v>128.13311365692499</v>
@@ -5658,7 +5659,7 @@
         <v>84</v>
       </c>
       <c r="AC52" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD52" s="1">
         <v>2</v>
@@ -5670,18 +5671,18 @@
         <v>0.05</v>
       </c>
       <c r="AI52" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D53" s="2">
         <v>130.40385095313701</v>
@@ -5747,7 +5748,7 @@
         <v>25</v>
       </c>
       <c r="AC53" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD53" s="1">
         <v>2</v>
@@ -5759,18 +5760,18 @@
         <v>0.05</v>
       </c>
       <c r="AI53" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D54" s="2">
         <v>137.778730455648</v>
@@ -5836,7 +5837,7 @@
         <v>47</v>
       </c>
       <c r="AC54" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD54" s="1">
         <v>2</v>
@@ -5848,18 +5849,18 @@
         <v>0.05</v>
       </c>
       <c r="AI54" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D55" s="2">
         <v>123.69781009649</v>
@@ -5925,7 +5926,7 @@
         <v>55</v>
       </c>
       <c r="AC55" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD55" s="1">
         <v>2</v>
@@ -5937,18 +5938,18 @@
         <v>0.05</v>
       </c>
       <c r="AI55" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D56" s="2">
         <v>134.72276664622899</v>
@@ -6014,7 +6015,7 @@
         <v>42</v>
       </c>
       <c r="AC56" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD56" s="1">
         <v>2</v>
@@ -6026,18 +6027,18 @@
         <v>0.05</v>
       </c>
       <c r="AI56" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D57" s="2">
         <v>134.33746914635</v>
@@ -6103,7 +6104,7 @@
         <v>25</v>
       </c>
       <c r="AC57" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD57" s="1">
         <v>2</v>
@@ -6115,18 +6116,18 @@
         <v>0.05</v>
       </c>
       <c r="AI57" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D58" s="2">
         <v>127.339688119233</v>
@@ -6192,7 +6193,7 @@
         <v>39</v>
       </c>
       <c r="AC58" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD58" s="1">
         <v>2</v>
@@ -6204,18 +6205,18 @@
         <v>0.05</v>
       </c>
       <c r="AI58" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D59" s="2">
         <v>126.928744047016</v>
@@ -6281,7 +6282,7 @@
         <v>33</v>
       </c>
       <c r="AC59" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD59" s="1">
         <v>2</v>
@@ -6293,18 +6294,18 @@
         <v>0.05</v>
       </c>
       <c r="AI59" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D60" s="2">
         <v>131.94108685129899</v>
@@ -6370,7 +6371,7 @@
         <v>23</v>
       </c>
       <c r="AC60" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD60" s="1">
         <v>2</v>
@@ -6382,18 +6383,18 @@
         <v>0.05</v>
       </c>
       <c r="AI60" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D61" s="2">
         <v>143.39858984460099</v>
@@ -6459,7 +6460,7 @@
         <v>47</v>
       </c>
       <c r="AC61" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD61" s="1">
         <v>2</v>
@@ -6471,18 +6472,18 @@
         <v>0.05</v>
       </c>
       <c r="AI61" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D62" s="2">
         <v>128.72544991966399</v>
@@ -6548,7 +6549,7 @@
         <v>92</v>
       </c>
       <c r="AC62" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD62" s="1">
         <v>2</v>
@@ -6560,18 +6561,18 @@
         <v>0.05</v>
       </c>
       <c r="AI62" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D63" s="2">
         <v>129.70518651958201</v>
@@ -6637,7 +6638,7 @@
         <v>92</v>
       </c>
       <c r="AC63" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD63" s="1">
         <v>2</v>
@@ -6649,18 +6650,18 @@
         <v>0.05</v>
       </c>
       <c r="AI63" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D64" s="2">
         <v>143.12034159811401</v>
@@ -6726,7 +6727,7 @@
         <v>29</v>
       </c>
       <c r="AC64" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD64" s="1">
         <v>2</v>
@@ -6738,18 +6739,18 @@
         <v>0.05</v>
       </c>
       <c r="AI64" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D65" s="2">
         <v>138.47893083658099</v>
@@ -6815,7 +6816,7 @@
         <v>55</v>
       </c>
       <c r="AC65" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD65" s="1">
         <v>2</v>
@@ -6827,18 +6828,18 @@
         <v>0.05</v>
       </c>
       <c r="AI65" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D66" s="2">
         <v>137.97679730060301</v>
@@ -6904,7 +6905,7 @@
         <v>112</v>
       </c>
       <c r="AC66" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD66" s="1">
         <v>2</v>
@@ -6916,18 +6917,18 @@
         <v>0.05</v>
       </c>
       <c r="AI66" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D67" s="2">
         <v>143.11017112236101</v>
@@ -6993,7 +6994,7 @@
         <v>83</v>
       </c>
       <c r="AC67" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD67" s="1">
         <v>2</v>
@@ -7005,18 +7006,18 @@
         <v>0.05</v>
       </c>
       <c r="AI67" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D68" s="2">
         <v>160.815433943557</v>
@@ -7082,7 +7083,7 @@
         <v>41</v>
       </c>
       <c r="AC68" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD68" s="1">
         <v>2</v>
@@ -7094,18 +7095,18 @@
         <v>0.05</v>
       </c>
       <c r="AI68" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D69" s="2">
         <v>151.32851202185</v>
@@ -7171,7 +7172,7 @@
         <v>24</v>
       </c>
       <c r="AC69" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD69" s="1">
         <v>2</v>
@@ -7183,18 +7184,18 @@
         <v>0.05</v>
       </c>
       <c r="AI69" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D70" s="2">
         <v>128.58090093466799</v>
@@ -7260,7 +7261,7 @@
         <v>87</v>
       </c>
       <c r="AC70" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD70" s="1">
         <v>2</v>
@@ -7272,18 +7273,18 @@
         <v>0.05</v>
       </c>
       <c r="AI70" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D71" s="2">
         <v>138.595456592147</v>
@@ -7349,7 +7350,7 @@
         <v>81</v>
       </c>
       <c r="AC71" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD71" s="1">
         <v>2</v>
@@ -7361,18 +7362,18 @@
         <v>0.05</v>
       </c>
       <c r="AI71" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D72" s="2">
         <v>143.24897819904399</v>
@@ -7438,7 +7439,7 @@
         <v>29</v>
       </c>
       <c r="AC72" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD72" s="1">
         <v>2</v>
@@ -7450,18 +7451,18 @@
         <v>0.05</v>
       </c>
       <c r="AI72" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D73" s="2">
         <v>156.0325133835</v>
@@ -7527,7 +7528,7 @@
         <v>32</v>
       </c>
       <c r="AC73" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD73" s="1">
         <v>2</v>
@@ -7539,18 +7540,18 @@
         <v>0.05</v>
       </c>
       <c r="AI73" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D74" s="2">
         <v>137.47948836192401</v>
@@ -7616,7 +7617,7 @@
         <v>19</v>
       </c>
       <c r="AC74" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD74" s="1">
         <v>2</v>
@@ -7628,18 +7629,18 @@
         <v>0.05</v>
       </c>
       <c r="AI74" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D75" s="2">
         <v>146.70645230993901</v>
@@ -7705,7 +7706,7 @@
         <v>85</v>
       </c>
       <c r="AC75" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD75" s="1">
         <v>2</v>
@@ -7717,18 +7718,18 @@
         <v>0.05</v>
       </c>
       <c r="AI75" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D76" s="2">
         <v>139.88391807975</v>
@@ -7794,7 +7795,7 @@
         <v>34</v>
       </c>
       <c r="AC76" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD76" s="1">
         <v>2</v>
@@ -7806,18 +7807,18 @@
         <v>0.05</v>
       </c>
       <c r="AI76" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D77" s="2">
         <v>144.94315998167801</v>
@@ -7883,7 +7884,7 @@
         <v>33</v>
       </c>
       <c r="AC77" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD77" s="1">
         <v>2</v>
@@ -7895,18 +7896,18 @@
         <v>0.05</v>
       </c>
       <c r="AI77" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D78" s="2">
         <v>129.80824935507999</v>
@@ -7972,7 +7973,7 @@
         <v>70</v>
       </c>
       <c r="AC78" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD78" s="1">
         <v>2</v>
@@ -7984,18 +7985,18 @@
         <v>0.05</v>
       </c>
       <c r="AI78" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D79" s="2">
         <v>136.246792352017</v>
@@ -8061,7 +8062,7 @@
         <v>49</v>
       </c>
       <c r="AC79" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD79" s="1">
         <v>2</v>
@@ -8073,18 +8074,18 @@
         <v>0.05</v>
       </c>
       <c r="AI79" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D80" s="2">
         <v>140.55609448526999</v>
@@ -8150,7 +8151,7 @@
         <v>29</v>
       </c>
       <c r="AC80" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD80" s="1">
         <v>2</v>
@@ -8162,18 +8163,18 @@
         <v>0.05</v>
       </c>
       <c r="AI80" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D81" s="2">
         <v>134.71148795728399</v>
@@ -8239,7 +8240,7 @@
         <v>52</v>
       </c>
       <c r="AC81" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD81" s="1">
         <v>2</v>
@@ -8251,18 +8252,18 @@
         <v>0.05</v>
       </c>
       <c r="AI81" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D82" s="2">
         <v>133.09824694102599</v>
@@ -8328,7 +8329,7 @@
         <v>35</v>
       </c>
       <c r="AC82" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD82" s="1">
         <v>2</v>
@@ -8340,18 +8341,18 @@
         <v>0.05</v>
       </c>
       <c r="AI82" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D83" s="2">
         <v>129.37537726382601</v>
@@ -8417,7 +8418,7 @@
         <v>46</v>
       </c>
       <c r="AC83" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD83" s="1">
         <v>2</v>
@@ -8429,18 +8430,18 @@
         <v>0.05</v>
       </c>
       <c r="AI83" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D84" s="2">
         <v>134.14124054860599</v>
@@ -8506,7 +8507,7 @@
         <v>100</v>
       </c>
       <c r="AC84" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD84" s="1">
         <v>2</v>
@@ -8518,18 +8519,18 @@
         <v>0.05</v>
       </c>
       <c r="AI84" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D85" s="2">
         <v>131.45551139320199</v>
@@ -8595,7 +8596,7 @@
         <v>67</v>
       </c>
       <c r="AC85" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD85" s="1">
         <v>2</v>
@@ -8607,18 +8608,18 @@
         <v>0.05</v>
       </c>
       <c r="AI85" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D86" s="2">
         <v>123.875103672108</v>
@@ -8684,7 +8685,7 @@
         <v>17</v>
       </c>
       <c r="AC86" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD86" s="1">
         <v>2</v>
@@ -8696,18 +8697,18 @@
         <v>0.05</v>
       </c>
       <c r="AI86" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D87" s="2">
         <v>113.882658025415</v>
@@ -8773,7 +8774,7 @@
         <v>31</v>
       </c>
       <c r="AC87" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD87" s="1">
         <v>2</v>
@@ -8785,18 +8786,18 @@
         <v>0.05</v>
       </c>
       <c r="AI87" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D88" s="2">
         <v>144.12109392985599</v>
@@ -8862,7 +8863,7 @@
         <v>84</v>
       </c>
       <c r="AC88" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD88" s="1">
         <v>2</v>
@@ -8874,18 +8875,18 @@
         <v>0.05</v>
       </c>
       <c r="AI88" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D89" s="2">
         <v>137.90707163322401</v>
@@ -8951,7 +8952,7 @@
         <v>24</v>
       </c>
       <c r="AC89" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AD89" s="1">
         <v>2</v>
@@ -8963,7 +8964,7 @@
         <v>0.05</v>
       </c>
       <c r="AI89" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>